<commit_message>
Profile class corresponds to a sheet of an ice core data spreadsheet.
Each profile of the profile class contains all the variable profile (e.g. salinity, conducitivity) of spreadsheet if non-null
</commit_message>
<xml_diff>
--- a/data_sample/ice_cores/testing-gap_extremity-TS.xlsx
+++ b/data_sample/ice_cores/testing-gap_extremity-TS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -692,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1011,8 +1011,8 @@
   </sheetPr>
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="C21 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1325,6 +1325,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1345,7 +1346,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="C21 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1463,7 +1464,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="1" sqref="C21 K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1490,7 +1491,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="1" sqref="C21 G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1652,7 +1653,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
+      <selection pane="topLeft" activeCell="F40" activeCellId="1" sqref="C21 F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1712,7 +1713,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="1" sqref="C21 C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>